<commit_message>
Histo consumption XLS: source/dest height + AMC columns width
</commit_message>
<xml_diff>
--- a/bin/addons/consumption_calculation/report/historical_consumption.xlsx
+++ b/bin/addons/consumption_calculation/report/historical_consumption.xlsx
@@ -679,15 +679,15 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="17" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1047,39 +1047,39 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="14.65" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.85546875" customWidth="1"/>
     <col min="2" max="2" width="28.140625" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
     <col min="4" max="5" width="17.7109375" customWidth="1"/>
     <col min="6" max="6" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="6">
         <v>43709</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="6">
         <v>43739</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="6">
         <v>43770</v>
       </c>
     </row>
@@ -1093,13 +1093,13 @@
       <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="7" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>